<commit_message>
Fixed U2, Added LEDs, downsized board dimensions, and general fixes
</commit_message>
<xml_diff>
--- a/BSPD/Project Outputs for BSPD/BSPD.xlsx
+++ b/BSPD/Project Outputs for BSPD/BSPD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faraz\Documents\Team Phantom\hardware\BSPD\Project Outputs for BSPD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E5F6298-F7D9-4F8B-9C55-C85FC14CBA71}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBABB35-9578-4011-A4E9-85FF8521DAD2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="960" windowWidth="14400" windowHeight="7360" xr2:uid="{DBD2FD9C-A994-4B39-9C18-3EF2A9EC72D8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{DBD2FD9C-A994-4B39-9C18-3EF2A9EC72D8}"/>
   </bookViews>
   <sheets>
     <sheet name="BSPD" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={55DEE6DD-6620-48EC-B2FC-50F2B2FCB8B0}</author>
+  </authors>
+  <commentList>
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{55DEE6DD-6620-48EC-B2FC-50F2B2FCB8B0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Currently on backorder, need to find a new combo with capacitor for RC Network; Tau = 0.5s</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
   <si>
     <t>Comment</t>
   </si>
@@ -272,13 +290,19 @@
   </si>
   <si>
     <t>1276-6456-1-ND</t>
+  </si>
+  <si>
+    <t>RC Network; Tau = 0.5s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,8 +310,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +327,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,12 +364,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -350,6 +391,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Faraz Borghei" id="{FC53DF5D-EE26-4F6C-8202-9271BC7CB911}" userId="Faraz Borghei" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,18 +694,28 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G6" dT="2019-03-22T01:53:32.76" personId="{FC53DF5D-EE26-4F6C-8202-9271BC7CB911}" id="{55DEE6DD-6620-48EC-B2FC-50F2B2FCB8B0}">
+    <text>Currently on backorder, need to find a new combo with capacitor for RC Network; Tau = 0.5s</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB1918B-B9B3-49C7-8297-71CACD817C24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB1918B-B9B3-49C7-8297-71CACD817C24}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
     <col min="2" max="3" width="14.26953125" customWidth="1"/>
     <col min="4" max="4" width="17.6328125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -782,25 +839,25 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -828,7 +885,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="A8" s="6">
         <v>499</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -989,31 +1046,42 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G20" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>